<commit_message>
Tests and documentation for fct_data_import
</commit_message>
<xml_diff>
--- a/inst/extdata/Plate_design.xlsx
+++ b/inst/extdata/Plate_design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsiekman\Documents\Brazillian_COVID_cohort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsiekman\Documents\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DAFA318-FA29-4F80-B7EA-215EADA5D0B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1852A9-7C87-45C9-BD1C-74734C5E2C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{640FE4C3-9150-49CA-984F-C3B2E4C26F7E}"/>
   </bookViews>
@@ -2034,10 +2034,13 @@
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="9.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>